<commit_message>
Adjust markov to newest InOutModule and LEGO
</commit_message>
<xml_diff>
--- a/data/markov/Global_Parameters.xlsx
+++ b/data/markov/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451B080A-484F-47FB-9728-7071140E477C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681268AC-50B4-4566-BD5F-1BFD3B90B040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34230" yWindow="-21705" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50190" yWindow="-21810" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>[h]</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Scaling factor for power values in input data (relative to 1MW)</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -803,25 +806,25 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="120.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.35546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="1"/>
+    <col min="6" max="6" width="120.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -841,7 +844,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -853,7 +856,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -873,12 +876,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -889,12 +892,12 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>9</v>
@@ -909,12 +912,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
@@ -924,7 +927,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
@@ -936,7 +939,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
@@ -956,12 +959,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
@@ -972,7 +975,7 @@
       <c r="F14" s="11"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
@@ -992,7 +995,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7" t="s">
         <v>5</v>
       </c>
@@ -1000,7 +1003,7 @@
       <c r="F17" s="12"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1014,7 @@
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1087,21 +1090,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1247,10 +1235,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1272,19 +1285,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update data/markov to newest formats
</commit_message>
<xml_diff>
--- a/data/markov/Global_Parameters.xlsx
+++ b/data/markov/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681268AC-50B4-4566-BD5F-1BFD3B90B040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE8C692-6350-4706-BD28-263EFBACDA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50190" yWindow="-21810" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>[h]</t>
   </si>
@@ -190,13 +190,19 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Format:</t>
+  </si>
+  <si>
+    <t>v0.1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -272,6 +278,11 @@
       <sz val="10"/>
       <name val="Aptos"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="8">
@@ -353,7 +364,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -402,6 +413,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -806,25 +823,33 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="120.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="120.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -844,7 +869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -856,7 +881,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -876,12 +901,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -892,7 +917,7 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -912,12 +937,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
@@ -927,7 +952,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
@@ -939,7 +964,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
@@ -959,12 +984,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
@@ -975,7 +1000,7 @@
       <c r="F14" s="11"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
@@ -995,7 +1020,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
         <v>5</v>
       </c>
@@ -1003,7 +1028,7 @@
       <c r="F17" s="12"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1014,7 +1039,7 @@
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1236,18 +1261,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1269,6 +1294,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1282,12 +1315,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>